<commit_message>
Updated Excel-version of the ANOVA-step-by-step-demonstration
</commit_message>
<xml_diff>
--- a/Analysis of variance/Clinical trial - Step-by-step.xlsx
+++ b/Analysis of variance/Clinical trial - Step-by-step.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="One-way ANOVA" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
     <author>SJ</author>
   </authors>
   <commentList>
-    <comment ref="G28" authorId="0">
+    <comment ref="H28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="40">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -242,11 +242,19 @@
     <r>
       <rPr>
         <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
-      <t xml:space="preserve">.1 </t>
+      <t xml:space="preserve">.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: no ther.</t>
     </r>
   </si>
   <si>
@@ -261,11 +269,19 @@
     <r>
       <rPr>
         <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
-      <t xml:space="preserve">.2 </t>
+      <t xml:space="preserve">.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: CBT</t>
     </r>
   </si>
   <si>
@@ -280,11 +296,92 @@
     <r>
       <rPr>
         <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
-      <t xml:space="preserve">..  </t>
+      <t xml:space="preserve">..</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: placebo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: anxifree</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Y</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: joyzepam</t>
     </r>
   </si>
   <si>
@@ -368,7 +465,7 @@
     <numFmt numFmtId="167" formatCode="0"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -459,8 +556,20 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF2323DC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00AE00"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -473,6 +582,12 @@
     </font>
     <font>
       <b val="true"/>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <vertAlign val="subscript"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -538,7 +653,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -647,7 +762,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -655,6 +770,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -663,7 +790,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -676,6 +803,36 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF168253"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF2A6099"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9211E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -687,7 +844,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF00AE00"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -732,7 +889,7 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF2323DC"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -740,14 +897,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O28" activeCellId="0" sqref="O28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1539,7 +1696,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1548,14 +1705,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1564,7 +1721,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="5.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,7 +1738,8 @@
         <v>3</v>
       </c>
       <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1598,8 +1756,12 @@
       <c r="D2" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="H2" s="0" t="s">
+      <c r="E2" s="15" t="n">
+        <f aca="false">(D2-H$9) ^ 2</f>
+        <v>0.146944444444444</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="I2" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1616,11 +1778,15 @@
       <c r="D3" s="15" t="n">
         <v>0.3</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="G3" s="0" t="s">
+      <c r="E3" s="15" t="n">
+        <f aca="false">(D3-H$9) ^ 2</f>
+        <v>0.340277777777777</v>
+      </c>
+      <c r="F3" s="26"/>
+      <c r="H3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1637,16 +1803,20 @@
       <c r="D4" s="15" t="n">
         <v>0.1</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="0" t="s">
+      <c r="E4" s="15" t="n">
+        <f aca="false">(D4-H$9) ^ 2</f>
+        <v>0.613611111111111</v>
+      </c>
+      <c r="F4" s="26"/>
+      <c r="G4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="23" t="n">
-        <f aca="false">AVERAGEIF(B$2:B$19, F4, D$2:D$19)</f>
+      <c r="H4" s="27" t="n">
+        <f aca="false">AVERAGEIF(B$2:B$19, G4, D$2:D$19)</f>
         <v>0.45</v>
       </c>
-      <c r="H4" s="23" t="n">
-        <f aca="false">COUNTIF(B$2:B$19, F4) * (G4-G$9) ^ 2</f>
+      <c r="I4" s="23" t="n">
+        <f aca="false">COUNTIF(B$2:B$19, G4) * (H4-H$9) ^ 2</f>
         <v>1.12666666666667</v>
       </c>
     </row>
@@ -1663,16 +1833,20 @@
       <c r="D5" s="15" t="n">
         <v>0.6</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="0" t="s">
+      <c r="E5" s="15" t="n">
+        <f aca="false">(D5-H$9) ^ 2</f>
+        <v>0.0802777777777776</v>
+      </c>
+      <c r="F5" s="26"/>
+      <c r="G5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="23" t="n">
-        <f aca="false">AVERAGEIF(B$2:B$19, F5, D$2:D$19)</f>
+      <c r="H5" s="27" t="n">
+        <f aca="false">AVERAGEIF(B$2:B$19, G5, D$2:D$19)</f>
         <v>0.716666666666667</v>
       </c>
-      <c r="H5" s="23" t="n">
-        <f aca="false">COUNTIF(B$2:B$19, F5) * (G5-G$9) ^ 2</f>
+      <c r="I5" s="23" t="n">
+        <f aca="false">COUNTIF(B$2:B$19, G5) * (H5-H$9) ^ 2</f>
         <v>0.166666666666667</v>
       </c>
     </row>
@@ -1689,19 +1863,23 @@
       <c r="D6" s="15" t="n">
         <v>0.4</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="0" t="s">
+      <c r="E6" s="15" t="n">
+        <f aca="false">(D6-H$9) ^ 2</f>
+        <v>0.233611111111111</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="23" t="n">
-        <f aca="false">AVERAGEIF(B$2:B$19, F6, D$2:D$19)</f>
+      <c r="H6" s="27" t="n">
+        <f aca="false">AVERAGEIF(B$2:B$19, G6, D$2:D$19)</f>
         <v>1.48333333333333</v>
       </c>
-      <c r="H6" s="23" t="n">
-        <f aca="false">COUNTIF(B$2:B$19, F6) * (G6-G$9) ^ 2</f>
+      <c r="I6" s="23" t="n">
+        <f aca="false">COUNTIF(B$2:B$19, G6) * (H6-H$9) ^ 2</f>
         <v>2.16</v>
       </c>
-      <c r="J6" s="27"/>
+      <c r="K6" s="28"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1716,19 +1894,23 @@
       <c r="D7" s="15" t="n">
         <v>0.2</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27" t="s">
+      <c r="E7" s="15" t="n">
+        <f aca="false">(D7-H$9) ^ 2</f>
+        <v>0.466944444444444</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="23" t="n">
-        <f aca="false">AVERAGEIF(C$2:C$19, F7, D$2:D$19)</f>
+      <c r="H7" s="29" t="n">
+        <f aca="false">AVERAGEIF(C$2:C$19, G7, D$2:D$19)</f>
         <v>0.722222222222222</v>
       </c>
-      <c r="H7" s="23" t="n">
-        <f aca="false">COUNTIF(C$2:C$19, F7) * (G7-G$9) ^ 2</f>
+      <c r="I7" s="23" t="n">
+        <f aca="false">COUNTIF(C$2:C$19, G7) * (H7-H$9) ^ 2</f>
         <v>0.233611111111111</v>
       </c>
-      <c r="J7" s="27"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1743,16 +1925,20 @@
       <c r="D8" s="15" t="n">
         <v>1.4</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27" t="s">
+      <c r="E8" s="15" t="n">
+        <f aca="false">(D8-H$9) ^ 2</f>
+        <v>0.266944444444445</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="23" t="n">
-        <f aca="false">AVERAGEIF(C$2:C$19, F8, D$2:D$19)</f>
+      <c r="H8" s="29" t="n">
+        <f aca="false">AVERAGEIF(C$2:C$19, G8, D$2:D$19)</f>
         <v>1.04444444444444</v>
       </c>
-      <c r="H8" s="23" t="n">
-        <f aca="false">COUNTIF(C$2:C$19, F8) * (G8-G$9) ^ 2</f>
+      <c r="I8" s="23" t="n">
+        <f aca="false">COUNTIF(C$2:C$19, G8) * (H8-H$9) ^ 2</f>
         <v>0.233611111111111</v>
       </c>
     </row>
@@ -1769,15 +1955,19 @@
       <c r="D9" s="15" t="n">
         <v>1.7</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="0" t="s">
+      <c r="E9" s="15" t="n">
+        <f aca="false">(D9-H$9) ^ 2</f>
+        <v>0.666944444444445</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="23" t="n">
+      <c r="H9" s="30" t="n">
         <f aca="false">AVERAGE(D$2:D$19)</f>
         <v>0.883333333333333</v>
       </c>
-      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1792,7 +1982,11 @@
       <c r="D10" s="15" t="n">
         <v>1.3</v>
       </c>
-      <c r="E10" s="26"/>
+      <c r="E10" s="15" t="n">
+        <f aca="false">(D10-H$9) ^ 2</f>
+        <v>0.173611111111111</v>
+      </c>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -1807,21 +2001,25 @@
       <c r="D11" s="15" t="n">
         <v>0.6</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28" t="s">
+      <c r="E11" s="15" t="n">
+        <f aca="false">(D11-H$9) ^ 2</f>
+        <v>0.0802777777777776</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="I11" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="J11" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="K11" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="28" t="s">
+      <c r="L11" s="31" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1838,28 +2036,32 @@
       <c r="D12" s="15" t="n">
         <v>0.9</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="28" t="s">
+      <c r="E12" s="15" t="n">
+        <f aca="false">(D12-H$9) ^ 2</f>
+        <v>0.000277777777777791</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="23" t="n">
-        <f aca="false">SUM(H4:H6)</f>
+      <c r="H12" s="23" t="n">
+        <f aca="false">SUM(I4:I6)</f>
         <v>3.45333333333333</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="I12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I12" s="23" t="n">
-        <f aca="false">G12/H12</f>
+      <c r="J12" s="23" t="n">
+        <f aca="false">H12/I12</f>
         <v>1.72666666666667</v>
       </c>
-      <c r="J12" s="23" t="n">
-        <f aca="false">I12/I$14</f>
+      <c r="K12" s="23" t="n">
+        <f aca="false">J12/J$14</f>
         <v>26.1490384615384</v>
       </c>
-      <c r="K12" s="29" t="n">
-        <f aca="false">_xlfn.F.DIST.RT(J12, H12, H$14)</f>
-        <v>1.87236162411551E-005</v>
+      <c r="L12" s="32" t="n">
+        <f aca="false">_xlfn.F.DIST.RT(K12, I12, I$14)</f>
+        <v>1.87236162411552E-005</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1875,27 +2077,31 @@
       <c r="D13" s="15" t="n">
         <v>0.3</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="28" t="s">
+      <c r="E13" s="15" t="n">
+        <f aca="false">(D13-H$9) ^ 2</f>
+        <v>0.340277777777777</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="23" t="n">
-        <f aca="false">SUM(H7:H8)</f>
+      <c r="H13" s="23" t="n">
+        <f aca="false">SUM(I7:I8)</f>
         <v>0.467222222222222</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="I13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="23" t="n">
-        <f aca="false">G13/H13</f>
+      <c r="J13" s="23" t="n">
+        <f aca="false">H13/I13</f>
         <v>0.467222222222222</v>
       </c>
-      <c r="J13" s="23" t="n">
-        <f aca="false">I13/I$14</f>
-        <v>7.07572115384613</v>
-      </c>
-      <c r="K13" s="29" t="n">
-        <f aca="false">_xlfn.F.DIST.RT(J13, H13,H$14)</f>
+      <c r="K13" s="23" t="n">
+        <f aca="false">J13/J$14</f>
+        <v>7.07572115384612</v>
+      </c>
+      <c r="L13" s="32" t="n">
+        <f aca="false">_xlfn.F.DIST.RT(K13, I13,I$14)</f>
         <v>0.0186602355173393</v>
       </c>
     </row>
@@ -1912,24 +2118,28 @@
       <c r="D14" s="15" t="n">
         <v>1.1</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="28" t="s">
+      <c r="E14" s="15" t="n">
+        <f aca="false">(D14-H$9) ^ 2</f>
+        <v>0.0469444444444446</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="23" t="n">
-        <f aca="false">D20-SUM(G12:G13)</f>
-        <v>0.924444444444448</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">COUNT(D2:D19) - H12-H13 - 1</f>
+      <c r="H14" s="23" t="n">
+        <f aca="false">D20-SUM(H12:H13)</f>
+        <v>0.924444444444449</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">COUNT(D2:D19) - I12-I13 - 1</f>
         <v>14</v>
       </c>
-      <c r="I14" s="23" t="n">
-        <f aca="false">G14/H14</f>
+      <c r="J14" s="23" t="n">
+        <f aca="false">H14/I14</f>
         <v>0.0660317460317463</v>
       </c>
-      <c r="J14" s="23"/>
       <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1944,7 +2154,11 @@
       <c r="D15" s="15" t="n">
         <v>0.8</v>
       </c>
-      <c r="E15" s="26"/>
+      <c r="E15" s="15" t="n">
+        <f aca="false">(D15-H$9) ^ 2</f>
+        <v>0.00694444444444438</v>
+      </c>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1959,11 +2173,15 @@
       <c r="D16" s="15" t="n">
         <v>1.2</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="G16" s="0" t="s">
+      <c r="E16" s="15" t="n">
+        <f aca="false">(D16-H$9) ^ 2</f>
+        <v>0.100277777777778</v>
+      </c>
+      <c r="F16" s="26"/>
+      <c r="H16" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="I16" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1980,16 +2198,20 @@
       <c r="D17" s="15" t="n">
         <v>1.8</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="0" t="s">
+      <c r="E17" s="15" t="n">
+        <f aca="false">(D17-H$9) ^ 2</f>
+        <v>0.840277777777779</v>
+      </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="23" t="n">
-        <f aca="false">G12 / D$20</f>
-        <v>0.712762297901617</v>
-      </c>
       <c r="H17" s="23" t="n">
-        <f aca="false">(G12 - H12 * I$14) / (D$20 + I$14)</f>
+        <f aca="false">H12 / E$20</f>
+        <v>0.712762297901616</v>
+      </c>
+      <c r="I17" s="23" t="n">
+        <f aca="false">(H12 - I12 * J$14) / (E$20 + J$14)</f>
         <v>0.676287593529306</v>
       </c>
     </row>
@@ -2006,17 +2228,21 @@
       <c r="D18" s="15" t="n">
         <v>1.3</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="0" t="s">
+      <c r="E18" s="15" t="n">
+        <f aca="false">(D18-H$9) ^ 2</f>
+        <v>0.173611111111111</v>
+      </c>
+      <c r="F18" s="26"/>
+      <c r="G18" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="23" t="n">
-        <f aca="false">G13 / D$20</f>
+      <c r="H18" s="23" t="n">
+        <f aca="false">H13 / E$20</f>
         <v>0.0964338951955051</v>
       </c>
-      <c r="H18" s="23" t="n">
-        <f aca="false">(G13 - H13 * I$14) / (D$20 + I$14)</f>
-        <v>0.0816916886181095</v>
+      <c r="I18" s="23" t="n">
+        <f aca="false">(H13 - I13 * J$14) / (E$20 + J$14)</f>
+        <v>0.0816916886181094</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,13 +2258,17 @@
       <c r="D19" s="15" t="n">
         <v>1.4</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="G19" s="23" t="n">
-        <f aca="false">(G12 + G13) / D$20</f>
-        <v>0.809196193097122</v>
-      </c>
+      <c r="E19" s="15" t="n">
+        <f aca="false">(D19-H$9) ^ 2</f>
+        <v>0.266944444444445</v>
+      </c>
+      <c r="F19" s="26"/>
       <c r="H19" s="23" t="n">
-        <f aca="false">((G12+ G13) - (H12+H13) * I$14) / (D$20 +I$14)</f>
+        <f aca="false">(H12 + H13) / E$20</f>
+        <v>0.809196193097121</v>
+      </c>
+      <c r="I19" s="23" t="n">
+        <f aca="false">((H12+ H13) - (I12+I13) * J$14) / (E$20 +J$14)</f>
         <v>0.757979282147416</v>
       </c>
     </row>
@@ -2050,306 +2280,316 @@
         <f aca="false">_xlfn.VAR.P(D2:D19) * COUNT(D2:D19)</f>
         <v>4.845</v>
       </c>
-      <c r="E20" s="19"/>
+      <c r="E20" s="19" t="n">
+        <f aca="false">SUM(E2:E19)</f>
+        <v>4.845</v>
+      </c>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="19" t="s">
+      <c r="G21" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G22" s="0" t="s">
+    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H22" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="0" t="s">
+      <c r="I22" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="J22" s="33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="30" t="s">
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="23" t="n">
+      <c r="H23" s="23" t="n">
+        <f aca="false">AVERAGE(D2:D4)</f>
         <v>0.3</v>
       </c>
-      <c r="H23" s="23" t="n">
+      <c r="I23" s="23" t="n">
+        <f aca="false">AVERAGE(D11:D13)</f>
         <v>0.6</v>
       </c>
-      <c r="I23" s="23" t="n">
-        <f aca="false">G4</f>
+      <c r="J23" s="27" t="n">
+        <f aca="false">AVERAGE(H23:I23)</f>
         <v>0.45</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="30" t="s">
+    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="23" t="n">
+      <c r="H24" s="23" t="n">
+        <f aca="false">AVERAGE(D5:D7)</f>
         <v>0.4</v>
       </c>
-      <c r="H24" s="23" t="n">
-        <v>1.033333</v>
-      </c>
       <c r="I24" s="23" t="n">
-        <f aca="false">G5</f>
+        <f aca="false">AVERAGE(D14:D16)</f>
+        <v>1.03333333333333</v>
+      </c>
+      <c r="J24" s="27" t="n">
+        <f aca="false">AVERAGE(H24:I24)</f>
         <v>0.716666666666667</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="30" t="s">
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="23" t="n">
-        <v>1.466667</v>
-      </c>
       <c r="H25" s="23" t="n">
+        <f aca="false">AVERAGE(D8:D10)</f>
+        <v>1.46666666666667</v>
+      </c>
+      <c r="I25" s="23" t="n">
+        <f aca="false">AVERAGE(D17:D19)</f>
         <v>1.5</v>
       </c>
-      <c r="I25" s="23" t="n">
-        <f aca="false">G6</f>
+      <c r="J25" s="27" t="n">
+        <f aca="false">AVERAGE(H25:I25)</f>
         <v>1.48333333333333</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="30" t="s">
+    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="23" t="n">
-        <f aca="false">G7</f>
+      <c r="H26" s="29" t="n">
+        <f aca="false">AVERAGE(H23:H25)</f>
         <v>0.722222222222222</v>
       </c>
-      <c r="H26" s="23" t="n">
-        <f aca="false">G8</f>
+      <c r="I26" s="29" t="n">
+        <f aca="false">AVERAGE(I23:I25)</f>
         <v>1.04444444444444</v>
       </c>
-      <c r="I26" s="23" t="n">
-        <f aca="false">G9</f>
+      <c r="J26" s="30" t="n">
+        <f aca="false">AVERAGE(J23:J25)</f>
         <v>0.883333333333333</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="30"/>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="G28" s="23" t="n">
-        <f aca="false">3 * (G23 - $I23 - G$26 + $I$26) ^ 2</f>
+      <c r="G28" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="23" t="n">
+        <f aca="false">3 * (H23 - $J23 - H$26 + $J$26) ^ 2</f>
+        <v>0.000370370370370368</v>
+      </c>
+      <c r="I28" s="23" t="n">
+        <f aca="false">3 * (I23 - $J23 - I$26 + $J$26) ^ 2</f>
         <v>0.000370370370370375</v>
       </c>
-      <c r="H28" s="23" t="n">
-        <f aca="false">3 * (H23 - $I23 - H$26 + $I$26) ^ 2</f>
-        <v>0.00037037037037036</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="23" t="n">
-        <f aca="false">3 * (G24 - $I24 - G$26 + $I$26) ^ 2</f>
+      <c r="G29" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="23" t="n">
+        <f aca="false">3 * (H24 - $J24 - H$26 + $J$26) ^ 2</f>
+        <v>0.0725925925925927</v>
+      </c>
+      <c r="I29" s="23" t="n">
+        <f aca="false">3 * (I24 - $J24 - I$26 + $J$26) ^ 2</f>
         <v>0.0725925925925926</v>
       </c>
-      <c r="H29" s="23" t="n">
-        <f aca="false">3 * (H24 - $I24 - H$26 + $I$26) ^ 2</f>
-        <v>0.0725922814818148</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" s="23" t="n">
-        <f aca="false">3 * (G25 - $I25 - G$26 + $I$26) ^ 2</f>
-        <v>0.0625928814818148</v>
+      <c r="G30" s="33" t="s">
+        <v>35</v>
       </c>
       <c r="H30" s="23" t="n">
-        <f aca="false">3 * (H25 - $I25 - H$26 + $I$26) ^ 2</f>
-        <v>0.0625925925925926</v>
+        <f aca="false">3 * (H25 - $J25 - H$26 + $J$26) ^ 2</f>
+        <v>0.0625925925925925</v>
+      </c>
+      <c r="I30" s="23" t="n">
+        <f aca="false">3 * (I25 - $J25 - I$26 + $J$26) ^ 2</f>
+        <v>0.0625925925925927</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="30"/>
-      <c r="G31" s="23" t="n">
-        <f aca="false">SUM(G28:H30)</f>
-        <v>0.271111088889555</v>
+      <c r="G31" s="33"/>
+      <c r="H31" s="23" t="n">
+        <f aca="false">SUM(H28:I30)</f>
+        <v>0.271111111111111</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="28"/>
-      <c r="G33" s="28" t="s">
+      <c r="G33" s="31"/>
+      <c r="H33" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="28" t="s">
+      <c r="I33" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="28" t="s">
+      <c r="J33" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="28" t="s">
+      <c r="K33" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="K33" s="28" t="s">
+      <c r="L33" s="31" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="28" t="s">
+      <c r="G34" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="G34" s="23" t="n">
-        <f aca="false">SUM(H4:H6)</f>
+      <c r="H34" s="23" t="n">
+        <f aca="false">SUM(I4:I6)</f>
         <v>3.45333333333333</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="I34" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I34" s="23" t="n">
-        <f aca="false">G34/H34</f>
+      <c r="J34" s="23" t="n">
+        <f aca="false">H34/I34</f>
         <v>1.72666666666667</v>
       </c>
-      <c r="J34" s="23" t="n">
-        <f aca="false">I34/I$37</f>
-        <v>31.7142846356009</v>
-      </c>
-      <c r="K34" s="29" t="n">
-        <f aca="false">_xlfn.F.DIST.RT(J34, H34, H$37)</f>
-        <v>1.62133312483917E-005</v>
+      <c r="K34" s="23" t="n">
+        <f aca="false">J34/J$37</f>
+        <v>31.7142857142856</v>
+      </c>
+      <c r="L34" s="32" t="n">
+        <f aca="false">_xlfn.F.DIST.RT(K34, I34, I$37)</f>
+        <v>1.62133284660397E-005</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F35" s="28" t="s">
+      <c r="G35" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="G35" s="23" t="n">
-        <f aca="false">SUM(H7:H8)</f>
+      <c r="H35" s="23" t="n">
+        <f aca="false">SUM(I7:I8)</f>
         <v>0.467222222222222</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="I35" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I35" s="23" t="n">
-        <f aca="false">G35/H35</f>
+      <c r="J35" s="23" t="n">
+        <f aca="false">H35/I35</f>
         <v>0.467222222222222</v>
       </c>
-      <c r="J35" s="23" t="n">
-        <f aca="false">I35/I$37</f>
-        <v>8.58163236117773</v>
-      </c>
-      <c r="K35" s="29" t="n">
-        <f aca="false">_xlfn.F.DIST.RT(J35, H35, H$37)</f>
-        <v>0.0126170459574237</v>
+      <c r="K35" s="23" t="n">
+        <f aca="false">J35/J$37</f>
+        <v>8.58163265306116</v>
+      </c>
+      <c r="L35" s="32" t="n">
+        <f aca="false">_xlfn.F.DIST.RT(K35, I35, I$37)</f>
+        <v>0.0126170447896561</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="G36" s="23" t="n">
-        <f aca="false">G31</f>
-        <v>0.271111088889555</v>
-      </c>
-      <c r="H36" s="0" t="n">
+      <c r="G36" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H36" s="23" t="n">
+        <f aca="false">H31</f>
+        <v>0.271111111111111</v>
+      </c>
+      <c r="I36" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I36" s="23" t="n">
-        <f aca="false">G36/H36</f>
-        <v>0.135555544444778</v>
-      </c>
       <c r="J36" s="23" t="n">
-        <f aca="false">I36/I$37</f>
-        <v>2.48979562960745</v>
-      </c>
-      <c r="K36" s="29" t="n">
-        <f aca="false">_xlfn.F.DIST.RT(J36, H36, H$37)</f>
-        <v>0.124601734340503</v>
-      </c>
-      <c r="Q36" s="29"/>
+        <f aca="false">H36/I36</f>
+        <v>0.135555555555556</v>
+      </c>
+      <c r="K36" s="23" t="n">
+        <f aca="false">J36/J$37</f>
+        <v>2.48979591836733</v>
+      </c>
+      <c r="L36" s="32" t="n">
+        <f aca="false">_xlfn.F.DIST.RT(K36, I36, I$37)</f>
+        <v>0.124601708912345</v>
+      </c>
+      <c r="R36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F37" s="28" t="s">
+      <c r="G37" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="23" t="n">
-        <f aca="false">D20-SUM(G34:G36)</f>
-        <v>0.653333355554889</v>
-      </c>
-      <c r="H37" s="0" t="n">
-        <f aca="false">COUNT(D2:D19) - H12 - H13 - H36 - 1</f>
+      <c r="H37" s="23" t="n">
+        <f aca="false">D20-SUM(H34:H36)</f>
+        <v>0.653333333333338</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <f aca="false">COUNT(D2:D19) - I12 - I13 - I36 - 1</f>
         <v>12</v>
       </c>
-      <c r="I37" s="23" t="n">
-        <f aca="false">G37/H37</f>
-        <v>0.0544444462962407</v>
-      </c>
-      <c r="J37" s="23"/>
+      <c r="J37" s="23" t="n">
+        <f aca="false">H37/I37</f>
+        <v>0.0544444444444448</v>
+      </c>
       <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G39" s="0" t="s">
+      <c r="H39" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="0" t="s">
+      <c r="I39" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="0" t="s">
+      <c r="G40" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="G40" s="23" t="n">
-        <f aca="false">G34 / D$20</f>
+      <c r="H40" s="23" t="n">
+        <f aca="false">H34 / D$20</f>
         <v>0.712762297901616</v>
       </c>
-      <c r="H40" s="23" t="n">
-        <f aca="false">(G34 - H34* I$14) / (D$20 + I$14)</f>
+      <c r="I40" s="23" t="n">
+        <f aca="false">(H34 - I34* J$14) / (D$20 + J$14)</f>
         <v>0.676287593529306</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F41" s="0" t="s">
+      <c r="G41" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="G41" s="23" t="n">
-        <f aca="false">G35 / D$20</f>
-        <v>0.0964338951955051</v>
-      </c>
       <c r="H41" s="23" t="n">
-        <f aca="false">(G35 - H35* I$14) / (D$20 + I$14)</f>
-        <v>0.0816916886181095</v>
+        <f aca="false">H35 / D$20</f>
+        <v>0.096433895195505</v>
+      </c>
+      <c r="I41" s="23" t="n">
+        <f aca="false">(H35 - I35* J$14) / (D$20 + J$14)</f>
+        <v>0.0816916886181094</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F42" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="G42" s="23" t="n">
-        <f aca="false">G36 / D$20</f>
-        <v>0.0559568810917554</v>
+      <c r="G42" s="33" t="s">
+        <v>36</v>
       </c>
       <c r="H42" s="23" t="n">
-        <f aca="false">(G36 - H36* I$14) / (D$20 + I$14)</f>
-        <v>0.0283133166342117</v>
+        <f aca="false">H36 / D$20</f>
+        <v>0.0559568856782479</v>
+      </c>
+      <c r="I42" s="23" t="n">
+        <f aca="false">(H36 - I36* J$14) / (D$20 + J$14)</f>
+        <v>0.0283133211590361</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G43" s="23" t="n">
-        <f aca="false">SUM(G34:G36) / D$20</f>
-        <v>0.865153074188877</v>
-      </c>
       <c r="H43" s="23" t="n">
-        <f aca="false">(SUM(G34:G36) - SUM(H34:H36) * I$14) / (D$20 +I$14)</f>
-        <v>0.786292598781628</v>
+        <f aca="false">SUM(H34:H36) / D$20</f>
+        <v>0.865153078775369</v>
+      </c>
+      <c r="I43" s="23" t="n">
+        <f aca="false">(SUM(H34:H36) - SUM(I34:I36) * J$14) / (D$20 +J$14)</f>
+        <v>0.786292603306452</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2359,7 +2599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2377,14 +2617,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>36</v>
+      <c r="A1" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,7 +2825,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>